<commit_message>
Ready for run CCP IM+DF=0.8 OK
</commit_message>
<xml_diff>
--- a/notebooks/res_tex.xlsx
+++ b/notebooks/res_tex.xlsx
@@ -74,7 +74,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="1">
-    <numFmt numFmtId="164" formatCode="0.000"/>
+    <numFmt numFmtId="164" formatCode="0.0E+00"/>
   </numFmts>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
@@ -101,7 +101,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="42">
+  <borders count="36">
     <border>
       <left/>
       <right/>
@@ -219,13 +219,43 @@
       <diagonal/>
     </border>
     <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left style="medium">
         <color indexed="64"/>
       </left>
       <right style="thin">
         <color indexed="64"/>
       </right>
-      <top style="medium">
+      <top style="thin">
         <color indexed="64"/>
       </top>
       <bottom style="thin">
@@ -237,73 +267,13 @@
       <left style="thin">
         <color indexed="64"/>
       </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="medium">
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
         <color indexed="64"/>
       </top>
       <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="medium">
         <color indexed="64"/>
       </bottom>
       <diagonal/>
@@ -477,187 +447,135 @@
       <diagonal/>
     </border>
     <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left/>
       <right style="thin">
         <color indexed="64"/>
       </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
       <top/>
       <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right/>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
         <color indexed="64"/>
       </bottom>
       <diagonal/>
@@ -666,7 +584,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="68">
+  <cellXfs count="65">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -704,25 +622,22 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="9" fontId="1" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
@@ -731,142 +646,136 @@
     <xf numFmtId="2" fontId="0" fillId="0" borderId="18" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="19" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="19" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="20" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="21" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="9" fontId="1" fillId="0" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="22" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="23" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="27" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="28" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="29" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="30" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="23" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="24" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="31" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="32" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="33" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="35" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="34" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="22" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="20" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="25" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="18" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="22" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="28" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="30" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="31" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="31" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="32" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="33" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="34" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="34" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="35" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="24" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="25" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="26" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="29" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="36" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="37" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="38" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="39" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="40" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="41" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1192,15 +1101,14 @@
   <dimension ref="A1:V35"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L7" sqref="L7"/>
+      <selection activeCell="L10" sqref="L10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="10" width="8.7265625" style="1"/>
-    <col min="11" max="11" width="10" style="1" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="10.7265625" style="1" bestFit="1" customWidth="1"/>
-    <col min="13" max="16384" width="8.7265625" style="1"/>
+    <col min="1" max="3" width="11.7265625" style="1"/>
+    <col min="4" max="4" width="11.7265625" style="45"/>
+    <col min="5" max="16384" width="11.7265625" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:16" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
@@ -1209,69 +1117,71 @@
         <v>10</v>
       </c>
       <c r="B2" s="58"/>
-      <c r="C2" s="55" t="s">
+      <c r="C2" s="62" t="s">
         <v>15</v>
       </c>
-      <c r="D2" s="56"/>
-      <c r="E2" s="56"/>
-      <c r="F2" s="57"/>
-      <c r="G2" s="56" t="s">
+      <c r="D2" s="60"/>
+      <c r="E2" s="60"/>
+      <c r="F2" s="61"/>
+      <c r="G2" s="60" t="s">
         <v>16</v>
       </c>
-      <c r="H2" s="56"/>
-      <c r="I2" s="56"/>
-      <c r="J2" s="57"/>
+      <c r="H2" s="60"/>
+      <c r="I2" s="60"/>
+      <c r="J2" s="61"/>
       <c r="K2" s="2"/>
       <c r="L2" s="2"/>
-      <c r="M2" s="54"/>
-      <c r="N2" s="54"/>
-      <c r="O2" s="54"/>
-      <c r="P2" s="54"/>
+      <c r="M2" s="64"/>
+      <c r="N2" s="64"/>
+      <c r="O2" s="64"/>
+      <c r="P2" s="64"/>
     </row>
     <row r="3" spans="1:16" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B3" s="59"/>
-      <c r="C3" s="31" t="s">
+      <c r="C3" s="26" t="s">
         <v>0</v>
       </c>
-      <c r="D3" s="32" t="s">
+      <c r="D3" s="46" t="s">
         <v>7</v>
       </c>
-      <c r="E3" s="32" t="s">
+      <c r="E3" s="27" t="s">
         <v>9</v>
       </c>
-      <c r="F3" s="33" t="s">
+      <c r="F3" s="28" t="s">
         <v>8</v>
       </c>
-      <c r="G3" s="31" t="s">
+      <c r="G3" s="26" t="s">
         <v>0</v>
       </c>
-      <c r="H3" s="32" t="s">
+      <c r="H3" s="27" t="s">
         <v>7</v>
       </c>
-      <c r="I3" s="32" t="s">
+      <c r="I3" s="27" t="s">
         <v>9</v>
       </c>
-      <c r="J3" s="33" t="s">
+      <c r="J3" s="28" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="4" spans="1:16" x14ac:dyDescent="0.35">
-      <c r="B4" s="60" t="s">
+      <c r="B4" s="40" t="s">
         <v>1</v>
       </c>
-      <c r="C4" s="37">
+      <c r="C4" s="54">
         <v>2.3495916591100001E-2</v>
       </c>
-      <c r="D4" s="22"/>
-      <c r="E4" s="23"/>
-      <c r="F4" s="24"/>
-      <c r="G4" s="21"/>
-      <c r="H4" s="22"/>
-      <c r="I4" s="23"/>
-      <c r="J4" s="24"/>
+      <c r="D4" s="48"/>
+      <c r="E4" s="19"/>
+      <c r="F4" s="20"/>
+      <c r="G4" s="54">
+        <v>2.7763306592800002E-2</v>
+      </c>
+      <c r="H4" s="18"/>
+      <c r="I4" s="19"/>
+      <c r="J4" s="20"/>
       <c r="K4" s="3"/>
       <c r="L4" s="3"/>
-      <c r="M4" s="54"/>
+      <c r="M4" s="64"/>
       <c r="N4" s="4"/>
       <c r="O4" s="3"/>
       <c r="P4" s="3"/>
@@ -1280,37 +1190,41 @@
       <c r="B5" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="C5" s="38">
+      <c r="C5" s="55">
         <v>2.3606979556499999E-2</v>
       </c>
-      <c r="D5" s="11"/>
+      <c r="D5" s="49"/>
       <c r="E5" s="9"/>
-      <c r="F5" s="16"/>
-      <c r="G5" s="15"/>
+      <c r="F5" s="14"/>
+      <c r="G5" s="55">
+        <v>2.27692137737E-2</v>
+      </c>
       <c r="H5" s="11"/>
       <c r="I5" s="9"/>
-      <c r="J5" s="16"/>
+      <c r="J5" s="14"/>
       <c r="K5" s="3"/>
       <c r="L5" s="3"/>
-      <c r="M5" s="54"/>
+      <c r="M5" s="64"/>
       <c r="N5" s="5"/>
       <c r="O5" s="3"/>
       <c r="P5" s="3"/>
     </row>
     <row r="6" spans="1:16" x14ac:dyDescent="0.35">
-      <c r="B6" s="61" t="s">
+      <c r="B6" s="41" t="s">
         <v>3</v>
       </c>
-      <c r="C6" s="38">
+      <c r="C6" s="55">
         <v>6.0981043523300003E-3</v>
       </c>
-      <c r="D6" s="10"/>
+      <c r="D6" s="49"/>
       <c r="E6" s="9"/>
-      <c r="F6" s="16"/>
-      <c r="G6" s="15"/>
+      <c r="F6" s="14"/>
+      <c r="G6" s="55">
+        <v>6.6698576600000004E-3</v>
+      </c>
       <c r="H6" s="10"/>
       <c r="I6" s="9"/>
-      <c r="J6" s="16"/>
+      <c r="J6" s="14"/>
       <c r="K6" s="3"/>
       <c r="L6" s="3"/>
       <c r="N6" s="4"/>
@@ -1318,19 +1232,21 @@
       <c r="P6" s="3"/>
     </row>
     <row r="7" spans="1:16" x14ac:dyDescent="0.35">
-      <c r="B7" s="62" t="s">
+      <c r="B7" s="42" t="s">
         <v>6</v>
       </c>
-      <c r="C7" s="38">
+      <c r="C7" s="55">
         <v>1.2764280236300001</v>
       </c>
-      <c r="D7" s="10"/>
+      <c r="D7" s="49"/>
       <c r="E7" s="9"/>
-      <c r="F7" s="16"/>
-      <c r="G7" s="15"/>
+      <c r="F7" s="14"/>
+      <c r="G7" s="55">
+        <v>1.2003775007899999</v>
+      </c>
       <c r="H7" s="10"/>
       <c r="I7" s="9"/>
-      <c r="J7" s="16"/>
+      <c r="J7" s="14"/>
       <c r="K7" s="3"/>
       <c r="L7" s="3"/>
       <c r="N7" s="4"/>
@@ -1338,19 +1254,21 @@
       <c r="P7" s="3"/>
     </row>
     <row r="8" spans="1:16" x14ac:dyDescent="0.35">
-      <c r="B8" s="62" t="s">
+      <c r="B8" s="42" t="s">
         <v>4</v>
       </c>
-      <c r="C8" s="38">
+      <c r="C8" s="55">
         <v>1.6363098251099999</v>
       </c>
-      <c r="D8" s="10"/>
+      <c r="D8" s="49"/>
       <c r="E8" s="9"/>
-      <c r="F8" s="16"/>
-      <c r="G8" s="15"/>
+      <c r="F8" s="14"/>
+      <c r="G8" s="55">
+        <v>1.5504298350000001</v>
+      </c>
       <c r="H8" s="10"/>
       <c r="I8" s="9"/>
-      <c r="J8" s="16"/>
+      <c r="J8" s="14"/>
       <c r="K8" s="3"/>
       <c r="L8" s="3"/>
       <c r="N8" s="4"/>
@@ -1361,16 +1279,18 @@
       <c r="B9" s="8" t="s">
         <v>5</v>
       </c>
-      <c r="C9" s="39">
+      <c r="C9" s="56">
         <v>1.8030792276000001</v>
       </c>
-      <c r="D9" s="26"/>
-      <c r="E9" s="25"/>
-      <c r="F9" s="30"/>
-      <c r="G9" s="29"/>
-      <c r="H9" s="26"/>
-      <c r="I9" s="25"/>
-      <c r="J9" s="30"/>
+      <c r="D9" s="50"/>
+      <c r="E9" s="21"/>
+      <c r="F9" s="25"/>
+      <c r="G9" s="56">
+        <v>1.71326494826</v>
+      </c>
+      <c r="H9" s="22"/>
+      <c r="I9" s="21"/>
+      <c r="J9" s="25"/>
       <c r="K9" s="3"/>
       <c r="L9" s="3"/>
       <c r="N9" s="4"/>
@@ -1378,59 +1298,77 @@
       <c r="P9" s="3"/>
     </row>
     <row r="10" spans="1:16" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B10" s="35" t="s">
+      <c r="B10" s="30" t="s">
         <v>12</v>
       </c>
-      <c r="C10" s="67">
-        <f>SUM(C$4:C$6, C7)</f>
+      <c r="C10" s="51">
+        <f t="shared" ref="C10:D12" si="0">SUM(C$4:C$6, C7)</f>
         <v>1.32962902412993</v>
       </c>
-      <c r="D10" s="27"/>
-      <c r="E10" s="28"/>
-      <c r="F10" s="14"/>
-      <c r="G10" s="13"/>
-      <c r="H10" s="27"/>
-      <c r="I10" s="28"/>
-      <c r="J10" s="14"/>
+      <c r="D10" s="51">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="E10" s="24"/>
+      <c r="F10" s="13"/>
+      <c r="G10" s="51">
+        <f>SUM(G$4:G$6, G7)</f>
+        <v>1.2575798788165</v>
+      </c>
+      <c r="H10" s="23"/>
+      <c r="I10" s="24"/>
+      <c r="J10" s="13"/>
       <c r="L10" s="3"/>
       <c r="N10" s="5"/>
       <c r="P10" s="3"/>
     </row>
     <row r="11" spans="1:16" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B11" s="41" t="s">
+      <c r="B11" s="32" t="s">
         <v>13</v>
       </c>
-      <c r="C11" s="50">
-        <f>SUM(C$4:C$6, C8)</f>
+      <c r="C11" s="52">
+        <f t="shared" si="0"/>
         <v>1.6895108256099298</v>
       </c>
-      <c r="D11" s="40"/>
+      <c r="D11" s="52">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
       <c r="E11" s="12"/>
-      <c r="F11" s="16"/>
-      <c r="G11" s="15"/>
+      <c r="F11" s="14"/>
+      <c r="G11" s="52">
+        <f>SUM(G$4:G$6, G8)</f>
+        <v>1.6076322130265002</v>
+      </c>
       <c r="H11" s="11"/>
       <c r="I11" s="12"/>
-      <c r="J11" s="16"/>
+      <c r="J11" s="14"/>
       <c r="L11" s="3"/>
       <c r="M11" s="3"/>
       <c r="N11" s="5"/>
       <c r="P11" s="3"/>
     </row>
     <row r="12" spans="1:16" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B12" s="36" t="s">
+      <c r="B12" s="31" t="s">
         <v>14</v>
       </c>
-      <c r="C12" s="66">
-        <f>SUM(C$4:C$6, C9)</f>
+      <c r="C12" s="53">
+        <f t="shared" si="0"/>
         <v>1.85628022809993</v>
       </c>
-      <c r="D12" s="18"/>
-      <c r="E12" s="19"/>
-      <c r="F12" s="20"/>
-      <c r="G12" s="17"/>
-      <c r="H12" s="18"/>
-      <c r="I12" s="19"/>
-      <c r="J12" s="20"/>
+      <c r="D12" s="53">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="E12" s="16"/>
+      <c r="F12" s="17"/>
+      <c r="G12" s="53">
+        <f>SUM(G$4:G$6, G9)</f>
+        <v>1.7704673262865001</v>
+      </c>
+      <c r="H12" s="15"/>
+      <c r="I12" s="16"/>
+      <c r="J12" s="17"/>
       <c r="L12" s="3"/>
       <c r="M12" s="3"/>
       <c r="N12" s="5"/>
@@ -1438,7 +1376,7 @@
     </row>
     <row r="13" spans="1:16" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="C13" s="3"/>
-      <c r="D13" s="5"/>
+      <c r="D13" s="47"/>
       <c r="F13" s="3"/>
       <c r="G13" s="3"/>
       <c r="I13" s="3"/>
@@ -1453,18 +1391,18 @@
         <v>11</v>
       </c>
       <c r="B14" s="58"/>
-      <c r="C14" s="55" t="s">
+      <c r="C14" s="62" t="s">
         <v>15</v>
       </c>
-      <c r="D14" s="56"/>
-      <c r="E14" s="56"/>
-      <c r="F14" s="57"/>
-      <c r="G14" s="56" t="s">
+      <c r="D14" s="60"/>
+      <c r="E14" s="60"/>
+      <c r="F14" s="61"/>
+      <c r="G14" s="60" t="s">
         <v>16</v>
       </c>
-      <c r="H14" s="56"/>
-      <c r="I14" s="56"/>
-      <c r="J14" s="57"/>
+      <c r="H14" s="60"/>
+      <c r="I14" s="60"/>
+      <c r="J14" s="61"/>
       <c r="L14" s="3"/>
       <c r="M14" s="3"/>
       <c r="N14" s="5"/>
@@ -1472,28 +1410,28 @@
     </row>
     <row r="15" spans="1:16" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B15" s="59"/>
-      <c r="C15" s="31" t="s">
+      <c r="C15" s="26" t="s">
         <v>0</v>
       </c>
-      <c r="D15" s="32" t="s">
+      <c r="D15" s="46" t="s">
         <v>7</v>
       </c>
-      <c r="E15" s="32" t="s">
+      <c r="E15" s="27" t="s">
         <v>9</v>
       </c>
-      <c r="F15" s="33" t="s">
+      <c r="F15" s="28" t="s">
         <v>8</v>
       </c>
-      <c r="G15" s="31" t="s">
+      <c r="G15" s="26" t="s">
         <v>0</v>
       </c>
-      <c r="H15" s="32" t="s">
+      <c r="H15" s="27" t="s">
         <v>7</v>
       </c>
-      <c r="I15" s="32" t="s">
+      <c r="I15" s="27" t="s">
         <v>9</v>
       </c>
-      <c r="J15" s="33" t="s">
+      <c r="J15" s="28" t="s">
         <v>8</v>
       </c>
       <c r="L15" s="3"/>
@@ -1505,111 +1443,123 @@
       <c r="B16" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="C16" s="37">
+      <c r="C16" s="54">
         <v>4.8531774067800001E-2</v>
       </c>
-      <c r="D16" s="22"/>
-      <c r="E16" s="23"/>
-      <c r="F16" s="24"/>
-      <c r="G16" s="21"/>
-      <c r="H16" s="22"/>
-      <c r="I16" s="23"/>
-      <c r="J16" s="24"/>
+      <c r="D16" s="48"/>
+      <c r="E16" s="19"/>
+      <c r="F16" s="20"/>
+      <c r="G16" s="54">
+        <v>4.6170115497600001E-2</v>
+      </c>
+      <c r="H16" s="18"/>
+      <c r="I16" s="19"/>
+      <c r="J16" s="20"/>
       <c r="L16" s="3"/>
       <c r="M16" s="3"/>
       <c r="N16" s="5"/>
       <c r="P16" s="3"/>
     </row>
     <row r="17" spans="2:22" x14ac:dyDescent="0.35">
-      <c r="B17" s="61" t="s">
+      <c r="B17" s="41" t="s">
         <v>2</v>
       </c>
-      <c r="C17" s="38">
+      <c r="C17" s="55">
         <v>9.6998909585900003E-2</v>
       </c>
-      <c r="D17" s="11"/>
+      <c r="D17" s="49"/>
       <c r="E17" s="9"/>
-      <c r="F17" s="16"/>
-      <c r="G17" s="15"/>
+      <c r="F17" s="14"/>
+      <c r="G17" s="55">
+        <v>9.5198856168199994E-2</v>
+      </c>
       <c r="H17" s="11"/>
       <c r="I17" s="9"/>
-      <c r="J17" s="16"/>
+      <c r="J17" s="14"/>
       <c r="L17" s="3"/>
       <c r="M17" s="3"/>
       <c r="N17" s="5"/>
       <c r="P17" s="3"/>
     </row>
     <row r="18" spans="2:22" x14ac:dyDescent="0.35">
-      <c r="B18" s="61" t="s">
+      <c r="B18" s="41" t="s">
         <v>3</v>
       </c>
-      <c r="C18" s="38">
+      <c r="C18" s="55">
         <v>0.39465586428999999</v>
       </c>
-      <c r="D18" s="10"/>
+      <c r="D18" s="49"/>
       <c r="E18" s="9"/>
-      <c r="F18" s="16"/>
-      <c r="G18" s="15"/>
+      <c r="F18" s="14"/>
+      <c r="G18" s="55">
+        <v>0.36300457144600001</v>
+      </c>
       <c r="H18" s="10"/>
       <c r="I18" s="9"/>
-      <c r="J18" s="16"/>
+      <c r="J18" s="14"/>
       <c r="L18" s="3"/>
       <c r="M18" s="3"/>
       <c r="N18" s="5"/>
       <c r="P18" s="3"/>
     </row>
     <row r="19" spans="2:22" x14ac:dyDescent="0.35">
-      <c r="B19" s="61" t="s">
+      <c r="B19" s="41" t="s">
         <v>6</v>
       </c>
-      <c r="C19" s="38">
+      <c r="C19" s="55">
         <v>2.3521391680799999E-2</v>
       </c>
-      <c r="D19" s="10"/>
+      <c r="D19" s="49"/>
       <c r="E19" s="9"/>
-      <c r="F19" s="16"/>
-      <c r="G19" s="15"/>
+      <c r="F19" s="14"/>
+      <c r="G19" s="55">
+        <v>2.3044249287099999E-2</v>
+      </c>
       <c r="H19" s="10"/>
       <c r="I19" s="9"/>
-      <c r="J19" s="16"/>
+      <c r="J19" s="14"/>
       <c r="L19" s="3"/>
       <c r="M19" s="3"/>
       <c r="N19" s="5"/>
       <c r="P19" s="3"/>
     </row>
     <row r="20" spans="2:22" x14ac:dyDescent="0.35">
-      <c r="B20" s="61" t="s">
+      <c r="B20" s="41" t="s">
         <v>4</v>
       </c>
-      <c r="C20" s="38">
+      <c r="C20" s="55">
         <v>2.0323059684899999E-2</v>
       </c>
-      <c r="D20" s="10"/>
+      <c r="D20" s="49"/>
       <c r="E20" s="9"/>
-      <c r="F20" s="16"/>
-      <c r="G20" s="15"/>
+      <c r="F20" s="14"/>
+      <c r="G20" s="55">
+        <v>1.98190123644E-2</v>
+      </c>
       <c r="H20" s="10"/>
       <c r="I20" s="9"/>
-      <c r="J20" s="16"/>
+      <c r="J20" s="14"/>
       <c r="L20" s="3"/>
       <c r="M20" s="3"/>
       <c r="N20" s="5"/>
       <c r="P20" s="3"/>
     </row>
     <row r="21" spans="2:22" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B21" s="63" t="s">
+      <c r="B21" s="43" t="s">
         <v>5</v>
       </c>
-      <c r="C21" s="39">
+      <c r="C21" s="56">
         <v>1.9192882335500001E-2</v>
       </c>
-      <c r="D21" s="26"/>
-      <c r="E21" s="25"/>
-      <c r="F21" s="30"/>
-      <c r="G21" s="29"/>
-      <c r="H21" s="26"/>
-      <c r="I21" s="25"/>
-      <c r="J21" s="30"/>
+      <c r="D21" s="50"/>
+      <c r="E21" s="21"/>
+      <c r="F21" s="25"/>
+      <c r="G21" s="56">
+        <v>1.86839073664E-2</v>
+      </c>
+      <c r="H21" s="22"/>
+      <c r="I21" s="21"/>
+      <c r="J21" s="25"/>
       <c r="L21" s="3"/>
       <c r="M21" s="3"/>
       <c r="N21" s="5"/>
@@ -1619,37 +1569,49 @@
       <c r="B22" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="C22" s="50">
+      <c r="C22" s="52">
         <f>SUM(C$16:C$18, C19)</f>
         <v>0.56370793962450005</v>
       </c>
-      <c r="D22" s="64"/>
-      <c r="E22" s="44"/>
-      <c r="F22" s="45"/>
-      <c r="G22" s="42"/>
-      <c r="H22" s="43"/>
-      <c r="I22" s="44"/>
-      <c r="J22" s="45"/>
+      <c r="D22" s="51">
+        <f>SUM(D$4:D$6, D19)</f>
+        <v>0</v>
+      </c>
+      <c r="E22" s="34"/>
+      <c r="F22" s="35"/>
+      <c r="G22" s="51">
+        <f>SUM(G$16:G$18, G19)</f>
+        <v>0.52741779239889997</v>
+      </c>
+      <c r="H22" s="33"/>
+      <c r="I22" s="34"/>
+      <c r="J22" s="35"/>
       <c r="L22" s="3"/>
       <c r="M22" s="3"/>
       <c r="N22" s="5"/>
       <c r="P22" s="3"/>
     </row>
     <row r="23" spans="2:22" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B23" s="34" t="s">
+      <c r="B23" s="29" t="s">
         <v>13</v>
       </c>
-      <c r="C23" s="50">
+      <c r="C23" s="52">
         <f>SUM(C$16:C$18, C20)</f>
         <v>0.56050960762860003</v>
       </c>
-      <c r="D23" s="65"/>
-      <c r="E23" s="32"/>
-      <c r="F23" s="52"/>
-      <c r="G23" s="50"/>
-      <c r="H23" s="51"/>
-      <c r="I23" s="32"/>
-      <c r="J23" s="52"/>
+      <c r="D23" s="52">
+        <f>SUM(D$4:D$6, D20)</f>
+        <v>0</v>
+      </c>
+      <c r="E23" s="27"/>
+      <c r="F23" s="39"/>
+      <c r="G23" s="51">
+        <f>SUM(G$16:G$18, G20)</f>
+        <v>0.52419255547619992</v>
+      </c>
+      <c r="H23" s="38"/>
+      <c r="I23" s="27"/>
+      <c r="J23" s="39"/>
       <c r="L23" s="3"/>
       <c r="M23" s="3"/>
       <c r="N23" s="5"/>
@@ -1659,17 +1621,23 @@
       <c r="B24" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="C24" s="66">
+      <c r="C24" s="53">
         <f>SUM(C$16:C$18, C21)</f>
         <v>0.55937943027920001</v>
       </c>
-      <c r="D24" s="51"/>
-      <c r="E24" s="48"/>
-      <c r="F24" s="49"/>
-      <c r="G24" s="46"/>
-      <c r="H24" s="47"/>
-      <c r="I24" s="48"/>
-      <c r="J24" s="49"/>
+      <c r="D24" s="53">
+        <f>SUM(D$4:D$6, D21)</f>
+        <v>0</v>
+      </c>
+      <c r="E24" s="36"/>
+      <c r="F24" s="37"/>
+      <c r="G24" s="57">
+        <f>SUM(G$16:G$18, G21)</f>
+        <v>0.52305745047819996</v>
+      </c>
+      <c r="H24" s="44"/>
+      <c r="I24" s="36"/>
+      <c r="J24" s="37"/>
       <c r="L24" s="3"/>
       <c r="M24" s="3"/>
       <c r="N24" s="5"/>
@@ -1677,26 +1645,26 @@
     </row>
     <row r="25" spans="2:22" x14ac:dyDescent="0.35">
       <c r="C25" s="3"/>
-      <c r="D25" s="5"/>
+      <c r="D25" s="47"/>
       <c r="F25" s="3"/>
       <c r="G25" s="3"/>
       <c r="M25" s="3"/>
     </row>
     <row r="26" spans="2:22" x14ac:dyDescent="0.35">
       <c r="C26" s="3"/>
-      <c r="D26" s="5"/>
+      <c r="D26" s="47"/>
       <c r="F26" s="3"/>
       <c r="G26" s="3"/>
     </row>
     <row r="27" spans="2:22" x14ac:dyDescent="0.35">
-      <c r="O27" s="53"/>
-      <c r="P27" s="53"/>
-      <c r="Q27" s="53"/>
-      <c r="R27" s="53"/>
-      <c r="S27" s="53"/>
-      <c r="T27" s="53"/>
-      <c r="U27" s="53"/>
-      <c r="V27" s="53"/>
+      <c r="O27" s="63"/>
+      <c r="P27" s="63"/>
+      <c r="Q27" s="63"/>
+      <c r="R27" s="63"/>
+      <c r="S27" s="63"/>
+      <c r="T27" s="63"/>
+      <c r="U27" s="63"/>
+      <c r="V27" s="63"/>
     </row>
     <row r="29" spans="2:22" x14ac:dyDescent="0.35">
       <c r="O29" s="3"/>
@@ -1754,25 +1722,26 @@
     </row>
     <row r="35" spans="3:22" x14ac:dyDescent="0.35">
       <c r="C35" s="3"/>
-      <c r="D35" s="5"/>
+      <c r="D35" s="47"/>
       <c r="E35" s="3"/>
       <c r="F35" s="3"/>
       <c r="G35" s="3"/>
     </row>
   </sheetData>
   <mergeCells count="10">
+    <mergeCell ref="O27:R27"/>
+    <mergeCell ref="S27:V27"/>
+    <mergeCell ref="M2:P2"/>
+    <mergeCell ref="C14:F14"/>
+    <mergeCell ref="M4:M5"/>
     <mergeCell ref="B2:B3"/>
     <mergeCell ref="B14:B15"/>
     <mergeCell ref="G14:J14"/>
     <mergeCell ref="C2:F2"/>
     <mergeCell ref="G2:J2"/>
-    <mergeCell ref="O27:R27"/>
-    <mergeCell ref="S27:V27"/>
-    <mergeCell ref="M2:P2"/>
-    <mergeCell ref="C14:F14"/>
-    <mergeCell ref="M4:M5"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
Run for CCP 1vs1 IM+DF=0.8 OK
</commit_message>
<xml_diff>
--- a/notebooks/res_tex.xlsx
+++ b/notebooks/res_tex.xlsx
@@ -1100,8 +1100,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:V35"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L10" sqref="L10"/>
+    <sheetView tabSelected="1" topLeftCell="B7" workbookViewId="0">
+      <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1170,7 +1170,9 @@
       <c r="C4" s="54">
         <v>2.3495916591100001E-2</v>
       </c>
-      <c r="D4" s="48"/>
+      <c r="D4" s="48">
+        <v>3.4752169999999999E-2</v>
+      </c>
       <c r="E4" s="19"/>
       <c r="F4" s="20"/>
       <c r="G4" s="54">
@@ -1193,7 +1195,9 @@
       <c r="C5" s="55">
         <v>2.3606979556499999E-2</v>
       </c>
-      <c r="D5" s="49"/>
+      <c r="D5" s="49">
+        <v>1.7350528802100001E-2</v>
+      </c>
       <c r="E5" s="9"/>
       <c r="F5" s="14"/>
       <c r="G5" s="55">
@@ -1216,7 +1220,9 @@
       <c r="C6" s="55">
         <v>6.0981043523300003E-3</v>
       </c>
-      <c r="D6" s="49"/>
+      <c r="D6" s="49">
+        <v>-4.72881790235E-2</v>
+      </c>
       <c r="E6" s="9"/>
       <c r="F6" s="14"/>
       <c r="G6" s="55">
@@ -1238,7 +1244,9 @@
       <c r="C7" s="55">
         <v>1.2764280236300001</v>
       </c>
-      <c r="D7" s="49"/>
+      <c r="D7" s="49">
+        <v>4.8482091164100002E-2</v>
+      </c>
       <c r="E7" s="9"/>
       <c r="F7" s="14"/>
       <c r="G7" s="55">
@@ -1260,7 +1268,9 @@
       <c r="C8" s="55">
         <v>1.6363098251099999</v>
       </c>
-      <c r="D8" s="49"/>
+      <c r="D8" s="49">
+        <v>5.5896077776400002E-2</v>
+      </c>
       <c r="E8" s="9"/>
       <c r="F8" s="14"/>
       <c r="G8" s="55">
@@ -1282,7 +1292,9 @@
       <c r="C9" s="56">
         <v>1.8030792276000001</v>
       </c>
-      <c r="D9" s="50"/>
+      <c r="D9" s="50">
+        <v>5.9203337897699999E-2</v>
+      </c>
       <c r="E9" s="21"/>
       <c r="F9" s="25"/>
       <c r="G9" s="56">
@@ -1307,7 +1319,7 @@
       </c>
       <c r="D10" s="51">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>5.3296610942700003E-2</v>
       </c>
       <c r="E10" s="24"/>
       <c r="F10" s="13"/>
@@ -1332,7 +1344,7 @@
       </c>
       <c r="D11" s="52">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>6.0710597555000002E-2</v>
       </c>
       <c r="E11" s="12"/>
       <c r="F11" s="14"/>
@@ -1358,7 +1370,7 @@
       </c>
       <c r="D12" s="53">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>6.40178576763E-2</v>
       </c>
       <c r="E12" s="16"/>
       <c r="F12" s="17"/>
@@ -1446,7 +1458,9 @@
       <c r="C16" s="54">
         <v>4.8531774067800001E-2</v>
       </c>
-      <c r="D16" s="48"/>
+      <c r="D16" s="48">
+        <v>0.13220419</v>
+      </c>
       <c r="E16" s="19"/>
       <c r="F16" s="20"/>
       <c r="G16" s="54">
@@ -1467,7 +1481,9 @@
       <c r="C17" s="55">
         <v>9.6998909585900003E-2</v>
       </c>
-      <c r="D17" s="49"/>
+      <c r="D17" s="49">
+        <v>0.11227771665400001</v>
+      </c>
       <c r="E17" s="9"/>
       <c r="F17" s="14"/>
       <c r="G17" s="55">
@@ -1488,7 +1504,9 @@
       <c r="C18" s="55">
         <v>0.39465586428999999</v>
       </c>
-      <c r="D18" s="49"/>
+      <c r="D18" s="49">
+        <v>-7.1482368162699997E-2</v>
+      </c>
       <c r="E18" s="9"/>
       <c r="F18" s="14"/>
       <c r="G18" s="55">
@@ -1509,8 +1527,9 @@
       <c r="C19" s="55">
         <v>2.3521391680799999E-2</v>
       </c>
-      <c r="D19" s="49"/>
-      <c r="E19" s="9"/>
+      <c r="D19" s="50">
+        <v>2.0876598874899999E-2</v>
+      </c>
       <c r="F19" s="14"/>
       <c r="G19" s="55">
         <v>2.3044249287099999E-2</v>
@@ -1530,7 +1549,9 @@
       <c r="C20" s="55">
         <v>2.0323059684899999E-2</v>
       </c>
-      <c r="D20" s="49"/>
+      <c r="D20" s="49">
+        <v>1.8959050098099998E-2</v>
+      </c>
       <c r="E20" s="9"/>
       <c r="F20" s="14"/>
       <c r="G20" s="55">
@@ -1551,7 +1572,9 @@
       <c r="C21" s="56">
         <v>1.9192882335500001E-2</v>
       </c>
-      <c r="D21" s="50"/>
+      <c r="D21" s="49">
+        <v>1.8172989473100001E-2</v>
+      </c>
       <c r="E21" s="21"/>
       <c r="F21" s="25"/>
       <c r="G21" s="56">
@@ -1574,8 +1597,8 @@
         <v>0.56370793962450005</v>
       </c>
       <c r="D22" s="51">
-        <f>SUM(D$4:D$6, D19)</f>
-        <v>0</v>
+        <f>SUM(D$4:D$6, D20)</f>
+        <v>2.3773569876699999E-2</v>
       </c>
       <c r="E22" s="34"/>
       <c r="F22" s="35"/>
@@ -1600,8 +1623,8 @@
         <v>0.56050960762860003</v>
       </c>
       <c r="D23" s="52">
-        <f>SUM(D$4:D$6, D20)</f>
-        <v>0</v>
+        <f>SUM(D$4:D$6, D21)</f>
+        <v>2.2987509251700001E-2</v>
       </c>
       <c r="E23" s="27"/>
       <c r="F23" s="39"/>
@@ -1626,8 +1649,8 @@
         <v>0.55937943027920001</v>
       </c>
       <c r="D24" s="53">
-        <f>SUM(D$4:D$6, D21)</f>
-        <v>0</v>
+        <f>SUM(D$4:D$6, D19)</f>
+        <v>2.56911186535E-2</v>
       </c>
       <c r="E24" s="36"/>
       <c r="F24" s="37"/>

</xml_diff>

<commit_message>
Run CCP 1vs1 DF = 0.05xIM OK
</commit_message>
<xml_diff>
--- a/notebooks/res_tex.xlsx
+++ b/notebooks/res_tex.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="18">
   <si>
     <t>Bilat</t>
   </si>
@@ -68,6 +68,9 @@
   <si>
     <t>n=8</t>
   </si>
+  <si>
+    <t>CCP 0.05</t>
+  </si>
 </sst>
 </file>
 
@@ -584,7 +587,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="65">
+  <cellXfs count="72">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -757,25 +760,46 @@
     <xf numFmtId="164" fontId="0" fillId="0" borderId="25" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="11" fontId="0" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="11" fontId="0" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="11" fontId="0" fillId="0" borderId="19" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="19" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1100,8 +1124,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:V35"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B7" workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E24" sqref="E24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1116,28 +1140,28 @@
       <c r="A2" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="B2" s="58"/>
-      <c r="C2" s="62" t="s">
+      <c r="B2" s="63"/>
+      <c r="C2" s="60" t="s">
         <v>15</v>
       </c>
-      <c r="D2" s="60"/>
-      <c r="E2" s="60"/>
-      <c r="F2" s="61"/>
-      <c r="G2" s="60" t="s">
+      <c r="D2" s="61"/>
+      <c r="E2" s="61"/>
+      <c r="F2" s="62"/>
+      <c r="G2" s="61" t="s">
         <v>16</v>
       </c>
-      <c r="H2" s="60"/>
-      <c r="I2" s="60"/>
-      <c r="J2" s="61"/>
+      <c r="H2" s="61"/>
+      <c r="I2" s="61"/>
+      <c r="J2" s="62"/>
       <c r="K2" s="2"/>
       <c r="L2" s="2"/>
-      <c r="M2" s="64"/>
-      <c r="N2" s="64"/>
-      <c r="O2" s="64"/>
-      <c r="P2" s="64"/>
+      <c r="M2" s="59"/>
+      <c r="N2" s="59"/>
+      <c r="O2" s="59"/>
+      <c r="P2" s="59"/>
     </row>
     <row r="3" spans="1:16" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B3" s="59"/>
+      <c r="B3" s="64"/>
       <c r="C3" s="26" t="s">
         <v>0</v>
       </c>
@@ -1145,7 +1169,7 @@
         <v>7</v>
       </c>
       <c r="E3" s="27" t="s">
-        <v>9</v>
+        <v>17</v>
       </c>
       <c r="F3" s="28" t="s">
         <v>8</v>
@@ -1173,7 +1197,9 @@
       <c r="D4" s="48">
         <v>3.4752169999999999E-2</v>
       </c>
-      <c r="E4" s="19"/>
+      <c r="E4" s="68">
+        <v>3.3233119999999998E-2</v>
+      </c>
       <c r="F4" s="20"/>
       <c r="G4" s="54">
         <v>2.7763306592800002E-2</v>
@@ -1183,7 +1209,7 @@
       <c r="J4" s="20"/>
       <c r="K4" s="3"/>
       <c r="L4" s="3"/>
-      <c r="M4" s="64"/>
+      <c r="M4" s="59"/>
       <c r="N4" s="4"/>
       <c r="O4" s="3"/>
       <c r="P4" s="3"/>
@@ -1198,7 +1224,9 @@
       <c r="D5" s="49">
         <v>1.7350528802100001E-2</v>
       </c>
-      <c r="E5" s="9"/>
+      <c r="E5" s="69">
+        <v>1.6467039109699998E-2</v>
+      </c>
       <c r="F5" s="14"/>
       <c r="G5" s="55">
         <v>2.27692137737E-2</v>
@@ -1208,7 +1236,7 @@
       <c r="J5" s="14"/>
       <c r="K5" s="3"/>
       <c r="L5" s="3"/>
-      <c r="M5" s="64"/>
+      <c r="M5" s="59"/>
       <c r="N5" s="5"/>
       <c r="O5" s="3"/>
       <c r="P5" s="3"/>
@@ -1223,7 +1251,9 @@
       <c r="D6" s="49">
         <v>-4.72881790235E-2</v>
       </c>
-      <c r="E6" s="9"/>
+      <c r="E6" s="69">
+        <v>-4.4013210490600002E-2</v>
+      </c>
       <c r="F6" s="14"/>
       <c r="G6" s="55">
         <v>6.6698576600000004E-3</v>
@@ -1247,7 +1277,9 @@
       <c r="D7" s="49">
         <v>4.8482091164100002E-2</v>
       </c>
-      <c r="E7" s="9"/>
+      <c r="E7" s="69">
+        <v>3.06136511821E-2</v>
+      </c>
       <c r="F7" s="14"/>
       <c r="G7" s="55">
         <v>1.2003775007899999</v>
@@ -1271,7 +1303,9 @@
       <c r="D8" s="49">
         <v>5.5896077776400002E-2</v>
       </c>
-      <c r="E8" s="9"/>
+      <c r="E8" s="69">
+        <v>3.6478073490399998E-2</v>
+      </c>
       <c r="F8" s="14"/>
       <c r="G8" s="55">
         <v>1.5504298350000001</v>
@@ -1295,7 +1329,9 @@
       <c r="D9" s="50">
         <v>5.9203337897699999E-2</v>
       </c>
-      <c r="E9" s="21"/>
+      <c r="E9" s="70">
+        <v>3.9035359232099998E-2</v>
+      </c>
       <c r="F9" s="25"/>
       <c r="G9" s="56">
         <v>1.71326494826</v>
@@ -1321,7 +1357,10 @@
         <f t="shared" si="0"/>
         <v>5.3296610942700003E-2</v>
       </c>
-      <c r="E10" s="24"/>
+      <c r="E10" s="51">
+        <f t="shared" ref="E10" si="1">SUM(E$4:E$6, E7)</f>
+        <v>3.6300599801199991E-2</v>
+      </c>
       <c r="F10" s="13"/>
       <c r="G10" s="51">
         <f>SUM(G$4:G$6, G7)</f>
@@ -1346,7 +1385,10 @@
         <f t="shared" si="0"/>
         <v>6.0710597555000002E-2</v>
       </c>
-      <c r="E11" s="12"/>
+      <c r="E11" s="52">
+        <f t="shared" ref="E11" si="2">SUM(E$4:E$6, E8)</f>
+        <v>4.2165022109499989E-2</v>
+      </c>
       <c r="F11" s="14"/>
       <c r="G11" s="52">
         <f>SUM(G$4:G$6, G8)</f>
@@ -1372,7 +1414,10 @@
         <f t="shared" si="0"/>
         <v>6.40178576763E-2</v>
       </c>
-      <c r="E12" s="16"/>
+      <c r="E12" s="53">
+        <f t="shared" ref="E12" si="3">SUM(E$4:E$6, E9)</f>
+        <v>4.4722307851199988E-2</v>
+      </c>
       <c r="F12" s="17"/>
       <c r="G12" s="53">
         <f>SUM(G$4:G$6, G9)</f>
@@ -1402,26 +1447,26 @@
       <c r="A14" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="B14" s="58"/>
-      <c r="C14" s="62" t="s">
+      <c r="B14" s="63"/>
+      <c r="C14" s="60" t="s">
         <v>15</v>
       </c>
-      <c r="D14" s="60"/>
-      <c r="E14" s="60"/>
-      <c r="F14" s="61"/>
-      <c r="G14" s="60" t="s">
+      <c r="D14" s="61"/>
+      <c r="E14" s="61"/>
+      <c r="F14" s="62"/>
+      <c r="G14" s="61" t="s">
         <v>16</v>
       </c>
-      <c r="H14" s="60"/>
-      <c r="I14" s="60"/>
-      <c r="J14" s="61"/>
+      <c r="H14" s="61"/>
+      <c r="I14" s="61"/>
+      <c r="J14" s="62"/>
       <c r="L14" s="3"/>
       <c r="M14" s="3"/>
       <c r="N14" s="5"/>
       <c r="P14" s="3"/>
     </row>
     <row r="15" spans="1:16" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B15" s="59"/>
+      <c r="B15" s="64"/>
       <c r="C15" s="26" t="s">
         <v>0</v>
       </c>
@@ -1429,7 +1474,7 @@
         <v>7</v>
       </c>
       <c r="E15" s="27" t="s">
-        <v>9</v>
+        <v>17</v>
       </c>
       <c r="F15" s="28" t="s">
         <v>8</v>
@@ -1461,7 +1506,9 @@
       <c r="D16" s="48">
         <v>0.13220419</v>
       </c>
-      <c r="E16" s="19"/>
+      <c r="E16" s="65">
+        <v>0.13491156000000001</v>
+      </c>
       <c r="F16" s="20"/>
       <c r="G16" s="54">
         <v>4.6170115497600001E-2</v>
@@ -1484,7 +1531,9 @@
       <c r="D17" s="49">
         <v>0.11227771665400001</v>
       </c>
-      <c r="E17" s="9"/>
+      <c r="E17" s="66">
+        <v>0.117693142446</v>
+      </c>
       <c r="F17" s="14"/>
       <c r="G17" s="55">
         <v>9.5198856168199994E-2</v>
@@ -1507,7 +1556,9 @@
       <c r="D18" s="49">
         <v>-7.1482368162699997E-2</v>
       </c>
-      <c r="E18" s="9"/>
+      <c r="E18" s="66">
+        <v>-7.7746089016799996E-2</v>
+      </c>
       <c r="F18" s="14"/>
       <c r="G18" s="55">
         <v>0.36300457144600001</v>
@@ -1530,6 +1581,9 @@
       <c r="D19" s="50">
         <v>2.0876598874899999E-2</v>
       </c>
+      <c r="E19" s="71">
+        <v>1.8186120736899999E-2</v>
+      </c>
       <c r="F19" s="14"/>
       <c r="G19" s="55">
         <v>2.3044249287099999E-2</v>
@@ -1552,7 +1606,9 @@
       <c r="D20" s="49">
         <v>1.8959050098099998E-2</v>
       </c>
-      <c r="E20" s="9"/>
+      <c r="E20" s="66">
+        <v>1.66486008633E-2</v>
+      </c>
       <c r="F20" s="14"/>
       <c r="G20" s="55">
         <v>1.98190123644E-2</v>
@@ -1575,7 +1631,9 @@
       <c r="D21" s="49">
         <v>1.8172989473100001E-2</v>
       </c>
-      <c r="E21" s="21"/>
+      <c r="E21" s="67">
+        <v>1.57842238641E-2</v>
+      </c>
       <c r="F21" s="25"/>
       <c r="G21" s="56">
         <v>1.86839073664E-2</v>
@@ -1596,11 +1654,14 @@
         <f>SUM(C$16:C$18, C19)</f>
         <v>0.56370793962450005</v>
       </c>
-      <c r="D22" s="51">
-        <f>SUM(D$4:D$6, D20)</f>
-        <v>2.3773569876699999E-2</v>
-      </c>
-      <c r="E22" s="34"/>
+      <c r="D22" s="52">
+        <f>SUM(D$16:D$18, D19)</f>
+        <v>0.19387613736620002</v>
+      </c>
+      <c r="E22" s="52">
+        <f>SUM(E$16:E$18, E19)</f>
+        <v>0.19304473416610002</v>
+      </c>
       <c r="F22" s="35"/>
       <c r="G22" s="51">
         <f>SUM(G$16:G$18, G19)</f>
@@ -1623,10 +1684,13 @@
         <v>0.56050960762860003</v>
       </c>
       <c r="D23" s="52">
-        <f>SUM(D$4:D$6, D21)</f>
-        <v>2.2987509251700001E-2</v>
-      </c>
-      <c r="E23" s="27"/>
+        <f>SUM(D$16:D$18, D20)</f>
+        <v>0.19195858858940001</v>
+      </c>
+      <c r="E23" s="52">
+        <f>SUM(E$16:E$18, E20)</f>
+        <v>0.19150721429250003</v>
+      </c>
       <c r="F23" s="39"/>
       <c r="G23" s="51">
         <f>SUM(G$16:G$18, G20)</f>
@@ -1649,10 +1713,13 @@
         <v>0.55937943027920001</v>
       </c>
       <c r="D24" s="53">
-        <f>SUM(D$4:D$6, D19)</f>
-        <v>2.56911186535E-2</v>
-      </c>
-      <c r="E24" s="36"/>
+        <f>SUM(D$16:D$18, D21)</f>
+        <v>0.19117252796440001</v>
+      </c>
+      <c r="E24" s="53">
+        <f>SUM(E$16:E$18, E21)</f>
+        <v>0.19064283729330003</v>
+      </c>
       <c r="F24" s="37"/>
       <c r="G24" s="57">
         <f>SUM(G$16:G$18, G21)</f>
@@ -1680,14 +1747,14 @@
       <c r="G26" s="3"/>
     </row>
     <row r="27" spans="2:22" x14ac:dyDescent="0.35">
-      <c r="O27" s="63"/>
-      <c r="P27" s="63"/>
-      <c r="Q27" s="63"/>
-      <c r="R27" s="63"/>
-      <c r="S27" s="63"/>
-      <c r="T27" s="63"/>
-      <c r="U27" s="63"/>
-      <c r="V27" s="63"/>
+      <c r="O27" s="58"/>
+      <c r="P27" s="58"/>
+      <c r="Q27" s="58"/>
+      <c r="R27" s="58"/>
+      <c r="S27" s="58"/>
+      <c r="T27" s="58"/>
+      <c r="U27" s="58"/>
+      <c r="V27" s="58"/>
     </row>
     <row r="29" spans="2:22" x14ac:dyDescent="0.35">
       <c r="O29" s="3"/>
@@ -1752,16 +1819,16 @@
     </row>
   </sheetData>
   <mergeCells count="10">
+    <mergeCell ref="B2:B3"/>
+    <mergeCell ref="B14:B15"/>
+    <mergeCell ref="G14:J14"/>
+    <mergeCell ref="C2:F2"/>
+    <mergeCell ref="G2:J2"/>
     <mergeCell ref="O27:R27"/>
     <mergeCell ref="S27:V27"/>
     <mergeCell ref="M2:P2"/>
     <mergeCell ref="C14:F14"/>
     <mergeCell ref="M4:M5"/>
-    <mergeCell ref="B2:B3"/>
-    <mergeCell ref="B14:B15"/>
-    <mergeCell ref="G14:J14"/>
-    <mergeCell ref="C2:F2"/>
-    <mergeCell ref="G2:J2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>

</xml_diff>

<commit_message>
Run CCP 1vs8 IM+DF=0.8
</commit_message>
<xml_diff>
--- a/notebooks/res_tex.xlsx
+++ b/notebooks/res_tex.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="19">
   <si>
     <t>Bilat</t>
   </si>
@@ -71,6 +71,9 @@
   <si>
     <t>CCP 0.05</t>
   </si>
+  <si>
+    <t>CCP 0.2</t>
+  </si>
 </sst>
 </file>
 
@@ -104,7 +107,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="36">
+  <borders count="35">
     <border>
       <left/>
       <right/>
@@ -572,22 +575,11 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left/>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="72">
+  <cellXfs count="63">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -616,12 +608,6 @@
     <xf numFmtId="2" fontId="0" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="9" fontId="1" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -631,18 +617,12 @@
     <xf numFmtId="2" fontId="0" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="9" fontId="1" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -652,12 +632,6 @@
     <xf numFmtId="2" fontId="0" fillId="0" borderId="19" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="9" fontId="1" fillId="0" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -685,9 +659,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="27" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -700,9 +671,6 @@
     <xf numFmtId="2" fontId="0" fillId="0" borderId="30" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="23" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="24" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -716,9 +684,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="33" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="35" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -1125,13 +1090,13 @@
   <dimension ref="A1:V35"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E24" sqref="E24"/>
+      <selection activeCell="L22" sqref="L22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="3" width="11.7265625" style="1"/>
-    <col min="4" max="4" width="11.7265625" style="45"/>
+    <col min="4" max="4" width="11.7265625" style="36"/>
     <col min="5" max="16384" width="11.7265625" style="1"/>
   </cols>
   <sheetData>
@@ -1140,76 +1105,78 @@
       <c r="A2" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="B2" s="63"/>
-      <c r="C2" s="60" t="s">
+      <c r="B2" s="54"/>
+      <c r="C2" s="51" t="s">
         <v>15</v>
       </c>
-      <c r="D2" s="61"/>
-      <c r="E2" s="61"/>
-      <c r="F2" s="62"/>
-      <c r="G2" s="61" t="s">
+      <c r="D2" s="52"/>
+      <c r="E2" s="52"/>
+      <c r="F2" s="53"/>
+      <c r="G2" s="52" t="s">
         <v>16</v>
       </c>
-      <c r="H2" s="61"/>
-      <c r="I2" s="61"/>
-      <c r="J2" s="62"/>
+      <c r="H2" s="52"/>
+      <c r="I2" s="52"/>
+      <c r="J2" s="53"/>
       <c r="K2" s="2"/>
       <c r="L2" s="2"/>
-      <c r="M2" s="59"/>
-      <c r="N2" s="59"/>
-      <c r="O2" s="59"/>
-      <c r="P2" s="59"/>
+      <c r="M2" s="50"/>
+      <c r="N2" s="50"/>
+      <c r="O2" s="50"/>
+      <c r="P2" s="50"/>
     </row>
     <row r="3" spans="1:16" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B3" s="64"/>
-      <c r="C3" s="26" t="s">
+      <c r="B3" s="55"/>
+      <c r="C3" s="20" t="s">
         <v>0</v>
       </c>
-      <c r="D3" s="46" t="s">
+      <c r="D3" s="37" t="s">
         <v>7</v>
       </c>
-      <c r="E3" s="27" t="s">
+      <c r="E3" s="21" t="s">
         <v>17</v>
       </c>
-      <c r="F3" s="28" t="s">
+      <c r="F3" s="22" t="s">
+        <v>18</v>
+      </c>
+      <c r="G3" s="20" t="s">
+        <v>0</v>
+      </c>
+      <c r="H3" s="21" t="s">
+        <v>7</v>
+      </c>
+      <c r="I3" s="21" t="s">
+        <v>9</v>
+      </c>
+      <c r="J3" s="22" t="s">
         <v>8</v>
       </c>
-      <c r="G3" s="26" t="s">
-        <v>0</v>
-      </c>
-      <c r="H3" s="27" t="s">
-        <v>7</v>
-      </c>
-      <c r="I3" s="27" t="s">
-        <v>9</v>
-      </c>
-      <c r="J3" s="28" t="s">
-        <v>8</v>
-      </c>
     </row>
     <row r="4" spans="1:16" x14ac:dyDescent="0.35">
-      <c r="B4" s="40" t="s">
+      <c r="B4" s="32" t="s">
         <v>1</v>
       </c>
-      <c r="C4" s="54">
+      <c r="C4" s="45">
         <v>2.3495916591100001E-2</v>
       </c>
-      <c r="D4" s="48">
+      <c r="D4" s="39">
         <v>3.4752169999999999E-2</v>
       </c>
-      <c r="E4" s="68">
+      <c r="E4" s="59">
         <v>3.3233119999999998E-2</v>
       </c>
-      <c r="F4" s="20"/>
-      <c r="G4" s="54">
+      <c r="F4" s="16"/>
+      <c r="G4" s="45">
         <v>2.7763306592800002E-2</v>
       </c>
-      <c r="H4" s="18"/>
-      <c r="I4" s="19"/>
-      <c r="J4" s="20"/>
+      <c r="H4" s="39">
+        <v>2.2848810000000001E-2</v>
+      </c>
+      <c r="I4" s="15"/>
+      <c r="J4" s="16"/>
       <c r="K4" s="3"/>
       <c r="L4" s="3"/>
-      <c r="M4" s="59"/>
+      <c r="M4" s="50"/>
       <c r="N4" s="4"/>
       <c r="O4" s="3"/>
       <c r="P4" s="3"/>
@@ -1218,49 +1185,53 @@
       <c r="B5" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="C5" s="55">
+      <c r="C5" s="46">
         <v>2.3606979556499999E-2</v>
       </c>
-      <c r="D5" s="49">
+      <c r="D5" s="40">
         <v>1.7350528802100001E-2</v>
       </c>
-      <c r="E5" s="69">
+      <c r="E5" s="60">
         <v>1.6467039109699998E-2</v>
       </c>
-      <c r="F5" s="14"/>
-      <c r="G5" s="55">
+      <c r="F5" s="12"/>
+      <c r="G5" s="46">
         <v>2.27692137737E-2</v>
       </c>
-      <c r="H5" s="11"/>
+      <c r="H5" s="40">
+        <v>1.7350528802100001E-2</v>
+      </c>
       <c r="I5" s="9"/>
-      <c r="J5" s="14"/>
+      <c r="J5" s="12"/>
       <c r="K5" s="3"/>
       <c r="L5" s="3"/>
-      <c r="M5" s="59"/>
+      <c r="M5" s="50"/>
       <c r="N5" s="5"/>
       <c r="O5" s="3"/>
       <c r="P5" s="3"/>
     </row>
     <row r="6" spans="1:16" x14ac:dyDescent="0.35">
-      <c r="B6" s="41" t="s">
+      <c r="B6" s="33" t="s">
         <v>3</v>
       </c>
-      <c r="C6" s="55">
+      <c r="C6" s="46">
         <v>6.0981043523300003E-3</v>
       </c>
-      <c r="D6" s="49">
+      <c r="D6" s="40">
         <v>-4.72881790235E-2</v>
       </c>
-      <c r="E6" s="69">
+      <c r="E6" s="60">
         <v>-4.4013210490600002E-2</v>
       </c>
-      <c r="F6" s="14"/>
-      <c r="G6" s="55">
+      <c r="F6" s="12"/>
+      <c r="G6" s="46">
         <v>6.6698576600000004E-3</v>
       </c>
-      <c r="H6" s="10"/>
+      <c r="H6" s="40">
+        <v>-4.72881790235E-2</v>
+      </c>
       <c r="I6" s="9"/>
-      <c r="J6" s="14"/>
+      <c r="J6" s="12"/>
       <c r="K6" s="3"/>
       <c r="L6" s="3"/>
       <c r="N6" s="4"/>
@@ -1268,25 +1239,27 @@
       <c r="P6" s="3"/>
     </row>
     <row r="7" spans="1:16" x14ac:dyDescent="0.35">
-      <c r="B7" s="42" t="s">
+      <c r="B7" s="34" t="s">
         <v>6</v>
       </c>
-      <c r="C7" s="55">
+      <c r="C7" s="46">
         <v>1.2764280236300001</v>
       </c>
-      <c r="D7" s="49">
+      <c r="D7" s="40">
         <v>4.8482091164100002E-2</v>
       </c>
-      <c r="E7" s="69">
+      <c r="E7" s="60">
         <v>3.06136511821E-2</v>
       </c>
-      <c r="F7" s="14"/>
-      <c r="G7" s="55">
+      <c r="F7" s="12"/>
+      <c r="G7" s="46">
         <v>1.2003775007899999</v>
       </c>
-      <c r="H7" s="10"/>
+      <c r="H7" s="40">
+        <v>4.86305416245E-2</v>
+      </c>
       <c r="I7" s="9"/>
-      <c r="J7" s="14"/>
+      <c r="J7" s="12"/>
       <c r="K7" s="3"/>
       <c r="L7" s="3"/>
       <c r="N7" s="4"/>
@@ -1294,25 +1267,27 @@
       <c r="P7" s="3"/>
     </row>
     <row r="8" spans="1:16" x14ac:dyDescent="0.35">
-      <c r="B8" s="42" t="s">
+      <c r="B8" s="34" t="s">
         <v>4</v>
       </c>
-      <c r="C8" s="55">
+      <c r="C8" s="46">
         <v>1.6363098251099999</v>
       </c>
-      <c r="D8" s="49">
+      <c r="D8" s="40">
         <v>5.5896077776400002E-2</v>
       </c>
-      <c r="E8" s="69">
+      <c r="E8" s="60">
         <v>3.6478073490399998E-2</v>
       </c>
-      <c r="F8" s="14"/>
-      <c r="G8" s="55">
+      <c r="F8" s="12"/>
+      <c r="G8" s="46">
         <v>1.5504298350000001</v>
       </c>
-      <c r="H8" s="10"/>
+      <c r="H8" s="40">
+        <v>5.6063585278600003E-2</v>
+      </c>
       <c r="I8" s="9"/>
-      <c r="J8" s="14"/>
+      <c r="J8" s="12"/>
       <c r="K8" s="3"/>
       <c r="L8" s="3"/>
       <c r="N8" s="4"/>
@@ -1323,22 +1298,24 @@
       <c r="B9" s="8" t="s">
         <v>5</v>
       </c>
-      <c r="C9" s="56">
+      <c r="C9" s="47">
         <v>1.8030792276000001</v>
       </c>
-      <c r="D9" s="50">
+      <c r="D9" s="41">
         <v>5.9203337897699999E-2</v>
       </c>
-      <c r="E9" s="70">
+      <c r="E9" s="61">
         <v>3.9035359232099998E-2</v>
       </c>
-      <c r="F9" s="25"/>
-      <c r="G9" s="56">
+      <c r="F9" s="19"/>
+      <c r="G9" s="47">
         <v>1.71326494826</v>
       </c>
-      <c r="H9" s="22"/>
-      <c r="I9" s="21"/>
-      <c r="J9" s="25"/>
+      <c r="H9" s="41">
+        <v>5.9377799963900003E-2</v>
+      </c>
+      <c r="I9" s="17"/>
+      <c r="J9" s="19"/>
       <c r="K9" s="3"/>
       <c r="L9" s="3"/>
       <c r="N9" s="4"/>
@@ -1346,86 +1323,95 @@
       <c r="P9" s="3"/>
     </row>
     <row r="10" spans="1:16" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B10" s="30" t="s">
+      <c r="B10" s="24" t="s">
         <v>12</v>
       </c>
-      <c r="C10" s="51">
+      <c r="C10" s="42">
         <f t="shared" ref="C10:D12" si="0">SUM(C$4:C$6, C7)</f>
         <v>1.32962902412993</v>
       </c>
-      <c r="D10" s="51">
+      <c r="D10" s="42">
         <f t="shared" si="0"/>
         <v>5.3296610942700003E-2</v>
       </c>
-      <c r="E10" s="51">
+      <c r="E10" s="42">
         <f t="shared" ref="E10" si="1">SUM(E$4:E$6, E7)</f>
         <v>3.6300599801199991E-2</v>
       </c>
-      <c r="F10" s="13"/>
-      <c r="G10" s="51">
+      <c r="F10" s="11"/>
+      <c r="G10" s="42">
         <f>SUM(G$4:G$6, G7)</f>
         <v>1.2575798788165</v>
       </c>
-      <c r="H10" s="23"/>
-      <c r="I10" s="24"/>
-      <c r="J10" s="13"/>
+      <c r="H10" s="42">
+        <f>SUM(H$4:H$6, H7)</f>
+        <v>4.1541701403099998E-2</v>
+      </c>
+      <c r="I10" s="18"/>
+      <c r="J10" s="11"/>
       <c r="L10" s="3"/>
       <c r="N10" s="5"/>
       <c r="P10" s="3"/>
     </row>
     <row r="11" spans="1:16" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B11" s="32" t="s">
+      <c r="B11" s="26" t="s">
         <v>13</v>
       </c>
-      <c r="C11" s="52">
+      <c r="C11" s="43">
         <f t="shared" si="0"/>
         <v>1.6895108256099298</v>
       </c>
-      <c r="D11" s="52">
+      <c r="D11" s="43">
         <f t="shared" si="0"/>
         <v>6.0710597555000002E-2</v>
       </c>
-      <c r="E11" s="52">
+      <c r="E11" s="43">
         <f t="shared" ref="E11" si="2">SUM(E$4:E$6, E8)</f>
         <v>4.2165022109499989E-2</v>
       </c>
-      <c r="F11" s="14"/>
-      <c r="G11" s="52">
+      <c r="F11" s="12"/>
+      <c r="G11" s="43">
         <f>SUM(G$4:G$6, G8)</f>
         <v>1.6076322130265002</v>
       </c>
-      <c r="H11" s="11"/>
-      <c r="I11" s="12"/>
-      <c r="J11" s="14"/>
+      <c r="H11" s="43">
+        <f>SUM(H$4:H$6, H8)</f>
+        <v>4.8974745057200002E-2</v>
+      </c>
+      <c r="I11" s="10"/>
+      <c r="J11" s="12"/>
       <c r="L11" s="3"/>
       <c r="M11" s="3"/>
       <c r="N11" s="5"/>
       <c r="P11" s="3"/>
     </row>
     <row r="12" spans="1:16" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B12" s="31" t="s">
+      <c r="B12" s="25" t="s">
         <v>14</v>
       </c>
-      <c r="C12" s="53">
+      <c r="C12" s="44">
         <f t="shared" si="0"/>
         <v>1.85628022809993</v>
       </c>
-      <c r="D12" s="53">
+      <c r="D12" s="44">
         <f t="shared" si="0"/>
         <v>6.40178576763E-2</v>
       </c>
-      <c r="E12" s="53">
+      <c r="E12" s="44">
         <f t="shared" ref="E12" si="3">SUM(E$4:E$6, E9)</f>
         <v>4.4722307851199988E-2</v>
       </c>
-      <c r="F12" s="17"/>
-      <c r="G12" s="53">
+      <c r="F12" s="14"/>
+      <c r="G12" s="44">
         <f>SUM(G$4:G$6, G9)</f>
         <v>1.7704673262865001</v>
       </c>
-      <c r="H12" s="15"/>
-      <c r="I12" s="16"/>
-      <c r="J12" s="17"/>
+      <c r="H12" s="43">
+        <f>SUM(H$4:H$6, H9)</f>
+        <v>5.2288959742500002E-2</v>
+      </c>
+      <c r="I12" s="13"/>
+      <c r="J12" s="14"/>
       <c r="L12" s="3"/>
       <c r="M12" s="3"/>
       <c r="N12" s="5"/>
@@ -1433,7 +1419,7 @@
     </row>
     <row r="13" spans="1:16" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="C13" s="3"/>
-      <c r="D13" s="47"/>
+      <c r="D13" s="38"/>
       <c r="F13" s="3"/>
       <c r="G13" s="3"/>
       <c r="I13" s="3"/>
@@ -1447,48 +1433,48 @@
       <c r="A14" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="B14" s="63"/>
-      <c r="C14" s="60" t="s">
+      <c r="B14" s="54"/>
+      <c r="C14" s="51" t="s">
         <v>15</v>
       </c>
-      <c r="D14" s="61"/>
-      <c r="E14" s="61"/>
-      <c r="F14" s="62"/>
-      <c r="G14" s="61" t="s">
+      <c r="D14" s="52"/>
+      <c r="E14" s="52"/>
+      <c r="F14" s="53"/>
+      <c r="G14" s="52" t="s">
         <v>16</v>
       </c>
-      <c r="H14" s="61"/>
-      <c r="I14" s="61"/>
-      <c r="J14" s="62"/>
+      <c r="H14" s="52"/>
+      <c r="I14" s="52"/>
+      <c r="J14" s="53"/>
       <c r="L14" s="3"/>
       <c r="M14" s="3"/>
       <c r="N14" s="5"/>
       <c r="P14" s="3"/>
     </row>
     <row r="15" spans="1:16" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B15" s="64"/>
-      <c r="C15" s="26" t="s">
+      <c r="B15" s="55"/>
+      <c r="C15" s="20" t="s">
         <v>0</v>
       </c>
-      <c r="D15" s="46" t="s">
+      <c r="D15" s="37" t="s">
         <v>7</v>
       </c>
-      <c r="E15" s="27" t="s">
+      <c r="E15" s="21" t="s">
         <v>17</v>
       </c>
-      <c r="F15" s="28" t="s">
-        <v>8</v>
-      </c>
-      <c r="G15" s="26" t="s">
+      <c r="F15" s="22" t="s">
+        <v>18</v>
+      </c>
+      <c r="G15" s="20" t="s">
         <v>0</v>
       </c>
-      <c r="H15" s="27" t="s">
+      <c r="H15" s="21" t="s">
         <v>7</v>
       </c>
-      <c r="I15" s="27" t="s">
+      <c r="I15" s="21" t="s">
         <v>9</v>
       </c>
-      <c r="J15" s="28" t="s">
+      <c r="J15" s="22" t="s">
         <v>8</v>
       </c>
       <c r="L15" s="3"/>
@@ -1500,147 +1486,159 @@
       <c r="B16" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="C16" s="54">
+      <c r="C16" s="45">
         <v>4.8531774067800001E-2</v>
       </c>
-      <c r="D16" s="48">
+      <c r="D16" s="39">
         <v>0.13220419</v>
       </c>
-      <c r="E16" s="65">
+      <c r="E16" s="56">
         <v>0.13491156000000001</v>
       </c>
-      <c r="F16" s="20"/>
-      <c r="G16" s="54">
+      <c r="F16" s="16"/>
+      <c r="G16" s="45">
         <v>4.6170115497600001E-2</v>
       </c>
-      <c r="H16" s="18"/>
-      <c r="I16" s="19"/>
-      <c r="J16" s="20"/>
+      <c r="H16" s="39">
+        <v>4.0408100000000002E-2</v>
+      </c>
+      <c r="I16" s="15"/>
+      <c r="J16" s="16"/>
       <c r="L16" s="3"/>
       <c r="M16" s="3"/>
       <c r="N16" s="5"/>
       <c r="P16" s="3"/>
     </row>
     <row r="17" spans="2:22" x14ac:dyDescent="0.35">
-      <c r="B17" s="41" t="s">
+      <c r="B17" s="33" t="s">
         <v>2</v>
       </c>
-      <c r="C17" s="55">
+      <c r="C17" s="46">
         <v>9.6998909585900003E-2</v>
       </c>
-      <c r="D17" s="49">
+      <c r="D17" s="40">
         <v>0.11227771665400001</v>
       </c>
-      <c r="E17" s="66">
+      <c r="E17" s="57">
         <v>0.117693142446</v>
       </c>
-      <c r="F17" s="14"/>
-      <c r="G17" s="55">
+      <c r="F17" s="12"/>
+      <c r="G17" s="46">
         <v>9.5198856168199994E-2</v>
       </c>
-      <c r="H17" s="11"/>
+      <c r="H17" s="40">
+        <v>0.11227771665400001</v>
+      </c>
       <c r="I17" s="9"/>
-      <c r="J17" s="14"/>
+      <c r="J17" s="12"/>
       <c r="L17" s="3"/>
       <c r="M17" s="3"/>
       <c r="N17" s="5"/>
       <c r="P17" s="3"/>
     </row>
     <row r="18" spans="2:22" x14ac:dyDescent="0.35">
-      <c r="B18" s="41" t="s">
+      <c r="B18" s="33" t="s">
         <v>3</v>
       </c>
-      <c r="C18" s="55">
+      <c r="C18" s="46">
         <v>0.39465586428999999</v>
       </c>
-      <c r="D18" s="49">
+      <c r="D18" s="40">
         <v>-7.1482368162699997E-2</v>
       </c>
-      <c r="E18" s="66">
+      <c r="E18" s="57">
         <v>-7.7746089016799996E-2</v>
       </c>
-      <c r="F18" s="14"/>
-      <c r="G18" s="55">
+      <c r="F18" s="12"/>
+      <c r="G18" s="46">
         <v>0.36300457144600001</v>
       </c>
-      <c r="H18" s="10"/>
+      <c r="H18" s="40">
+        <v>-7.1482368162699997E-2</v>
+      </c>
       <c r="I18" s="9"/>
-      <c r="J18" s="14"/>
+      <c r="J18" s="12"/>
       <c r="L18" s="3"/>
       <c r="M18" s="3"/>
       <c r="N18" s="5"/>
       <c r="P18" s="3"/>
     </row>
     <row r="19" spans="2:22" x14ac:dyDescent="0.35">
-      <c r="B19" s="41" t="s">
+      <c r="B19" s="33" t="s">
         <v>6</v>
       </c>
-      <c r="C19" s="55">
+      <c r="C19" s="46">
         <v>2.3521391680799999E-2</v>
       </c>
-      <c r="D19" s="50">
+      <c r="D19" s="41">
         <v>2.0876598874899999E-2</v>
       </c>
-      <c r="E19" s="71">
+      <c r="E19" s="62">
         <v>1.8186120736899999E-2</v>
       </c>
-      <c r="F19" s="14"/>
-      <c r="G19" s="55">
+      <c r="F19" s="12"/>
+      <c r="G19" s="46">
         <v>2.3044249287099999E-2</v>
       </c>
-      <c r="H19" s="10"/>
+      <c r="H19" s="40">
+        <v>2.0571619333300002E-2</v>
+      </c>
       <c r="I19" s="9"/>
-      <c r="J19" s="14"/>
+      <c r="J19" s="12"/>
       <c r="L19" s="3"/>
       <c r="M19" s="3"/>
       <c r="N19" s="5"/>
       <c r="P19" s="3"/>
     </row>
     <row r="20" spans="2:22" x14ac:dyDescent="0.35">
-      <c r="B20" s="41" t="s">
+      <c r="B20" s="33" t="s">
         <v>4</v>
       </c>
-      <c r="C20" s="55">
+      <c r="C20" s="46">
         <v>2.0323059684899999E-2</v>
       </c>
-      <c r="D20" s="49">
+      <c r="D20" s="40">
         <v>1.8959050098099998E-2</v>
       </c>
-      <c r="E20" s="66">
+      <c r="E20" s="57">
         <v>1.66486008633E-2</v>
       </c>
-      <c r="F20" s="14"/>
-      <c r="G20" s="55">
+      <c r="F20" s="12"/>
+      <c r="G20" s="46">
         <v>1.98190123644E-2</v>
       </c>
-      <c r="H20" s="10"/>
+      <c r="H20" s="40">
+        <v>1.8669712122800001E-2</v>
+      </c>
       <c r="I20" s="9"/>
-      <c r="J20" s="14"/>
+      <c r="J20" s="12"/>
       <c r="L20" s="3"/>
       <c r="M20" s="3"/>
       <c r="N20" s="5"/>
       <c r="P20" s="3"/>
     </row>
     <row r="21" spans="2:22" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B21" s="43" t="s">
+      <c r="B21" s="35" t="s">
         <v>5</v>
       </c>
-      <c r="C21" s="56">
+      <c r="C21" s="47">
         <v>1.9192882335500001E-2</v>
       </c>
-      <c r="D21" s="49">
+      <c r="D21" s="40">
         <v>1.8172989473100001E-2</v>
       </c>
-      <c r="E21" s="67">
+      <c r="E21" s="58">
         <v>1.57842238641E-2</v>
       </c>
-      <c r="F21" s="25"/>
-      <c r="G21" s="56">
+      <c r="F21" s="19"/>
+      <c r="G21" s="47">
         <v>1.86839073664E-2</v>
       </c>
-      <c r="H21" s="22"/>
-      <c r="I21" s="21"/>
-      <c r="J21" s="25"/>
+      <c r="H21" s="41">
+        <v>1.78875640249E-2</v>
+      </c>
+      <c r="I21" s="17"/>
+      <c r="J21" s="19"/>
       <c r="L21" s="3"/>
       <c r="M21" s="3"/>
       <c r="N21" s="5"/>
@@ -1650,55 +1648,61 @@
       <c r="B22" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="C22" s="52">
+      <c r="C22" s="43">
         <f>SUM(C$16:C$18, C19)</f>
         <v>0.56370793962450005</v>
       </c>
-      <c r="D22" s="52">
+      <c r="D22" s="43">
         <f>SUM(D$16:D$18, D19)</f>
         <v>0.19387613736620002</v>
       </c>
-      <c r="E22" s="52">
+      <c r="E22" s="43">
         <f>SUM(E$16:E$18, E19)</f>
         <v>0.19304473416610002</v>
       </c>
-      <c r="F22" s="35"/>
-      <c r="G22" s="51">
+      <c r="F22" s="28"/>
+      <c r="G22" s="42">
         <f>SUM(G$16:G$18, G19)</f>
         <v>0.52741779239889997</v>
       </c>
-      <c r="H22" s="33"/>
-      <c r="I22" s="34"/>
-      <c r="J22" s="35"/>
+      <c r="H22" s="42">
+        <f>SUM(H$16:H$18, H19)</f>
+        <v>0.1017750678246</v>
+      </c>
+      <c r="I22" s="27"/>
+      <c r="J22" s="28"/>
       <c r="L22" s="3"/>
       <c r="M22" s="3"/>
       <c r="N22" s="5"/>
       <c r="P22" s="3"/>
     </row>
     <row r="23" spans="2:22" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B23" s="29" t="s">
+      <c r="B23" s="23" t="s">
         <v>13</v>
       </c>
-      <c r="C23" s="52">
+      <c r="C23" s="43">
         <f>SUM(C$16:C$18, C20)</f>
         <v>0.56050960762860003</v>
       </c>
-      <c r="D23" s="52">
+      <c r="D23" s="43">
         <f>SUM(D$16:D$18, D20)</f>
         <v>0.19195858858940001</v>
       </c>
-      <c r="E23" s="52">
+      <c r="E23" s="43">
         <f>SUM(E$16:E$18, E20)</f>
         <v>0.19150721429250003</v>
       </c>
-      <c r="F23" s="39"/>
-      <c r="G23" s="51">
+      <c r="F23" s="31"/>
+      <c r="G23" s="42">
         <f>SUM(G$16:G$18, G20)</f>
         <v>0.52419255547619992</v>
       </c>
-      <c r="H23" s="38"/>
-      <c r="I23" s="27"/>
-      <c r="J23" s="39"/>
+      <c r="H23" s="42">
+        <f>SUM(H$16:H$18, H20)</f>
+        <v>9.9873160614099996E-2</v>
+      </c>
+      <c r="I23" s="21"/>
+      <c r="J23" s="31"/>
       <c r="L23" s="3"/>
       <c r="M23" s="3"/>
       <c r="N23" s="5"/>
@@ -1708,26 +1712,29 @@
       <c r="B24" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="C24" s="53">
+      <c r="C24" s="44">
         <f>SUM(C$16:C$18, C21)</f>
         <v>0.55937943027920001</v>
       </c>
-      <c r="D24" s="53">
+      <c r="D24" s="44">
         <f>SUM(D$16:D$18, D21)</f>
         <v>0.19117252796440001</v>
       </c>
-      <c r="E24" s="53">
+      <c r="E24" s="44">
         <f>SUM(E$16:E$18, E21)</f>
         <v>0.19064283729330003</v>
       </c>
-      <c r="F24" s="37"/>
-      <c r="G24" s="57">
+      <c r="F24" s="30"/>
+      <c r="G24" s="48">
         <f>SUM(G$16:G$18, G21)</f>
         <v>0.52305745047819996</v>
       </c>
-      <c r="H24" s="44"/>
-      <c r="I24" s="36"/>
-      <c r="J24" s="37"/>
+      <c r="H24" s="48">
+        <f>SUM(H$16:H$18, H21)</f>
+        <v>9.9091012516200005E-2</v>
+      </c>
+      <c r="I24" s="29"/>
+      <c r="J24" s="30"/>
       <c r="L24" s="3"/>
       <c r="M24" s="3"/>
       <c r="N24" s="5"/>
@@ -1735,26 +1742,26 @@
     </row>
     <row r="25" spans="2:22" x14ac:dyDescent="0.35">
       <c r="C25" s="3"/>
-      <c r="D25" s="47"/>
+      <c r="D25" s="38"/>
       <c r="F25" s="3"/>
       <c r="G25" s="3"/>
       <c r="M25" s="3"/>
     </row>
     <row r="26" spans="2:22" x14ac:dyDescent="0.35">
       <c r="C26" s="3"/>
-      <c r="D26" s="47"/>
+      <c r="D26" s="38"/>
       <c r="F26" s="3"/>
       <c r="G26" s="3"/>
     </row>
     <row r="27" spans="2:22" x14ac:dyDescent="0.35">
-      <c r="O27" s="58"/>
-      <c r="P27" s="58"/>
-      <c r="Q27" s="58"/>
-      <c r="R27" s="58"/>
-      <c r="S27" s="58"/>
-      <c r="T27" s="58"/>
-      <c r="U27" s="58"/>
-      <c r="V27" s="58"/>
+      <c r="O27" s="49"/>
+      <c r="P27" s="49"/>
+      <c r="Q27" s="49"/>
+      <c r="R27" s="49"/>
+      <c r="S27" s="49"/>
+      <c r="T27" s="49"/>
+      <c r="U27" s="49"/>
+      <c r="V27" s="49"/>
     </row>
     <row r="29" spans="2:22" x14ac:dyDescent="0.35">
       <c r="O29" s="3"/>
@@ -1812,7 +1819,7 @@
     </row>
     <row r="35" spans="3:22" x14ac:dyDescent="0.35">
       <c r="C35" s="3"/>
-      <c r="D35" s="47"/>
+      <c r="D35" s="38"/>
       <c r="E35" s="3"/>
       <c r="F35" s="3"/>
       <c r="G35" s="3"/>

</xml_diff>

<commit_message>
Run CCP 1vs1 DF = 0.2xIM OK
</commit_message>
<xml_diff>
--- a/notebooks/res_tex.xlsx
+++ b/notebooks/res_tex.xlsx
@@ -69,10 +69,10 @@
     <t>n=8</t>
   </si>
   <si>
-    <t>CCP 0.05</t>
+    <t>CCP 0,05</t>
   </si>
   <si>
-    <t>CCP 0.2</t>
+    <t>CCP 0,2</t>
   </si>
 </sst>
 </file>
@@ -579,7 +579,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="63">
+  <cellXfs count="68">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -725,46 +725,61 @@
     <xf numFmtId="164" fontId="0" fillId="0" borderId="25" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="11" fontId="0" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="11" fontId="0" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="11" fontId="0" fillId="0" borderId="19" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="19" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="11" fontId="0" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="11" fontId="0" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="11" fontId="0" fillId="0" borderId="19" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="19" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="24" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="18" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="21" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1089,15 +1104,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:V35"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L22" sqref="L22"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="F23" sqref="F23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="3" width="11.7265625" style="1"/>
     <col min="4" max="4" width="11.7265625" style="36"/>
-    <col min="5" max="16384" width="11.7265625" style="1"/>
+    <col min="5" max="5" width="11.7265625" style="1"/>
+    <col min="6" max="6" width="11.7265625" style="63"/>
+    <col min="7" max="16384" width="11.7265625" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:16" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
@@ -1105,28 +1122,28 @@
       <c r="A2" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="B2" s="54"/>
-      <c r="C2" s="51" t="s">
+      <c r="B2" s="56"/>
+      <c r="C2" s="60" t="s">
         <v>15</v>
       </c>
-      <c r="D2" s="52"/>
-      <c r="E2" s="52"/>
-      <c r="F2" s="53"/>
-      <c r="G2" s="52" t="s">
+      <c r="D2" s="58"/>
+      <c r="E2" s="58"/>
+      <c r="F2" s="59"/>
+      <c r="G2" s="58" t="s">
         <v>16</v>
       </c>
-      <c r="H2" s="52"/>
-      <c r="I2" s="52"/>
-      <c r="J2" s="53"/>
+      <c r="H2" s="58"/>
+      <c r="I2" s="58"/>
+      <c r="J2" s="59"/>
       <c r="K2" s="2"/>
       <c r="L2" s="2"/>
-      <c r="M2" s="50"/>
-      <c r="N2" s="50"/>
-      <c r="O2" s="50"/>
-      <c r="P2" s="50"/>
+      <c r="M2" s="62"/>
+      <c r="N2" s="62"/>
+      <c r="O2" s="62"/>
+      <c r="P2" s="62"/>
     </row>
     <row r="3" spans="1:16" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B3" s="55"/>
+      <c r="B3" s="57"/>
       <c r="C3" s="20" t="s">
         <v>0</v>
       </c>
@@ -1136,7 +1153,7 @@
       <c r="E3" s="21" t="s">
         <v>17</v>
       </c>
-      <c r="F3" s="22" t="s">
+      <c r="F3" s="64" t="s">
         <v>18</v>
       </c>
       <c r="G3" s="20" t="s">
@@ -1162,10 +1179,12 @@
       <c r="D4" s="39">
         <v>3.4752169999999999E-2</v>
       </c>
-      <c r="E4" s="59">
+      <c r="E4" s="52">
         <v>3.3233119999999998E-2</v>
       </c>
-      <c r="F4" s="16"/>
+      <c r="F4" s="65">
+        <v>2.8904740000000002E-2</v>
+      </c>
       <c r="G4" s="45">
         <v>2.7763306592800002E-2</v>
       </c>
@@ -1176,7 +1195,7 @@
       <c r="J4" s="16"/>
       <c r="K4" s="3"/>
       <c r="L4" s="3"/>
-      <c r="M4" s="50"/>
+      <c r="M4" s="62"/>
       <c r="N4" s="4"/>
       <c r="O4" s="3"/>
       <c r="P4" s="3"/>
@@ -1191,10 +1210,12 @@
       <c r="D5" s="40">
         <v>1.7350528802100001E-2</v>
       </c>
-      <c r="E5" s="60">
+      <c r="E5" s="53">
         <v>1.6467039109699998E-2</v>
       </c>
-      <c r="F5" s="12"/>
+      <c r="F5" s="66">
+        <v>1.4204913902799999E-2</v>
+      </c>
       <c r="G5" s="46">
         <v>2.27692137737E-2</v>
       </c>
@@ -1205,7 +1226,7 @@
       <c r="J5" s="12"/>
       <c r="K5" s="3"/>
       <c r="L5" s="3"/>
-      <c r="M5" s="50"/>
+      <c r="M5" s="62"/>
       <c r="N5" s="5"/>
       <c r="O5" s="3"/>
       <c r="P5" s="3"/>
@@ -1220,10 +1241,12 @@
       <c r="D6" s="40">
         <v>-4.72881790235E-2</v>
       </c>
-      <c r="E6" s="60">
+      <c r="E6" s="53">
         <v>-4.4013210490600002E-2</v>
       </c>
-      <c r="F6" s="12"/>
+      <c r="F6" s="66">
+        <v>-3.4188038306799999E-2</v>
+      </c>
       <c r="G6" s="46">
         <v>6.6698576600000004E-3</v>
       </c>
@@ -1248,10 +1271,12 @@
       <c r="D7" s="40">
         <v>4.8482091164100002E-2</v>
       </c>
-      <c r="E7" s="60">
+      <c r="E7" s="53">
         <v>3.06136511821E-2</v>
       </c>
-      <c r="F7" s="12"/>
+      <c r="F7" s="66">
+        <v>4.2245463328100002E-2</v>
+      </c>
       <c r="G7" s="46">
         <v>1.2003775007899999</v>
       </c>
@@ -1276,10 +1301,12 @@
       <c r="D8" s="40">
         <v>5.5896077776400002E-2</v>
       </c>
-      <c r="E8" s="60">
+      <c r="E8" s="53">
         <v>3.6478073490399998E-2</v>
       </c>
-      <c r="F8" s="12"/>
+      <c r="F8" s="66">
+        <v>4.9201648871600001E-2</v>
+      </c>
       <c r="G8" s="46">
         <v>1.5504298350000001</v>
       </c>
@@ -1304,10 +1331,12 @@
       <c r="D9" s="41">
         <v>5.9203337897699999E-2</v>
       </c>
-      <c r="E9" s="61">
+      <c r="E9" s="54">
         <v>3.9035359232099998E-2</v>
       </c>
-      <c r="F9" s="19"/>
+      <c r="F9" s="67">
+        <v>5.2206272136200001E-2</v>
+      </c>
       <c r="G9" s="47">
         <v>1.71326494826</v>
       </c>
@@ -1335,16 +1364,19 @@
         <v>5.3296610942700003E-2</v>
       </c>
       <c r="E10" s="42">
-        <f t="shared" ref="E10" si="1">SUM(E$4:E$6, E7)</f>
+        <f t="shared" ref="E10:F10" si="1">SUM(E$4:E$6, E7)</f>
         <v>3.6300599801199991E-2</v>
       </c>
-      <c r="F10" s="11"/>
+      <c r="F10" s="42">
+        <f t="shared" si="1"/>
+        <v>5.1167078924100003E-2</v>
+      </c>
       <c r="G10" s="42">
-        <f>SUM(G$4:G$6, G7)</f>
+        <f t="shared" ref="G10:H12" si="2">SUM(G$4:G$6, G7)</f>
         <v>1.2575798788165</v>
       </c>
       <c r="H10" s="42">
-        <f>SUM(H$4:H$6, H7)</f>
+        <f t="shared" si="2"/>
         <v>4.1541701403099998E-2</v>
       </c>
       <c r="I10" s="18"/>
@@ -1366,16 +1398,19 @@
         <v>6.0710597555000002E-2</v>
       </c>
       <c r="E11" s="43">
-        <f t="shared" ref="E11" si="2">SUM(E$4:E$6, E8)</f>
+        <f t="shared" ref="E11:F11" si="3">SUM(E$4:E$6, E8)</f>
         <v>4.2165022109499989E-2</v>
       </c>
-      <c r="F11" s="12"/>
+      <c r="F11" s="43">
+        <f t="shared" si="3"/>
+        <v>5.8123264467600001E-2</v>
+      </c>
       <c r="G11" s="43">
-        <f>SUM(G$4:G$6, G8)</f>
+        <f t="shared" si="2"/>
         <v>1.6076322130265002</v>
       </c>
       <c r="H11" s="43">
-        <f>SUM(H$4:H$6, H8)</f>
+        <f t="shared" si="2"/>
         <v>4.8974745057200002E-2</v>
       </c>
       <c r="I11" s="10"/>
@@ -1398,16 +1433,19 @@
         <v>6.40178576763E-2</v>
       </c>
       <c r="E12" s="44">
-        <f t="shared" ref="E12" si="3">SUM(E$4:E$6, E9)</f>
+        <f t="shared" ref="E12:F12" si="4">SUM(E$4:E$6, E9)</f>
         <v>4.4722307851199988E-2</v>
       </c>
-      <c r="F12" s="14"/>
+      <c r="F12" s="44">
+        <f t="shared" si="4"/>
+        <v>6.1127887732200001E-2</v>
+      </c>
       <c r="G12" s="44">
-        <f>SUM(G$4:G$6, G9)</f>
+        <f t="shared" si="2"/>
         <v>1.7704673262865001</v>
       </c>
       <c r="H12" s="43">
-        <f>SUM(H$4:H$6, H9)</f>
+        <f t="shared" si="2"/>
         <v>5.2288959742500002E-2</v>
       </c>
       <c r="I12" s="13"/>
@@ -1420,7 +1458,6 @@
     <row r="13" spans="1:16" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="C13" s="3"/>
       <c r="D13" s="38"/>
-      <c r="F13" s="3"/>
       <c r="G13" s="3"/>
       <c r="I13" s="3"/>
       <c r="J13" s="5"/>
@@ -1433,26 +1470,26 @@
       <c r="A14" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="B14" s="54"/>
-      <c r="C14" s="51" t="s">
+      <c r="B14" s="56"/>
+      <c r="C14" s="60" t="s">
         <v>15</v>
       </c>
-      <c r="D14" s="52"/>
-      <c r="E14" s="52"/>
-      <c r="F14" s="53"/>
-      <c r="G14" s="52" t="s">
+      <c r="D14" s="58"/>
+      <c r="E14" s="58"/>
+      <c r="F14" s="59"/>
+      <c r="G14" s="58" t="s">
         <v>16</v>
       </c>
-      <c r="H14" s="52"/>
-      <c r="I14" s="52"/>
-      <c r="J14" s="53"/>
+      <c r="H14" s="58"/>
+      <c r="I14" s="58"/>
+      <c r="J14" s="59"/>
       <c r="L14" s="3"/>
       <c r="M14" s="3"/>
       <c r="N14" s="5"/>
       <c r="P14" s="3"/>
     </row>
     <row r="15" spans="1:16" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B15" s="55"/>
+      <c r="B15" s="57"/>
       <c r="C15" s="20" t="s">
         <v>0</v>
       </c>
@@ -1462,7 +1499,7 @@
       <c r="E15" s="21" t="s">
         <v>17</v>
       </c>
-      <c r="F15" s="22" t="s">
+      <c r="F15" s="64" t="s">
         <v>18</v>
       </c>
       <c r="G15" s="20" t="s">
@@ -1492,10 +1529,12 @@
       <c r="D16" s="39">
         <v>0.13220419</v>
       </c>
-      <c r="E16" s="56">
+      <c r="E16" s="49">
         <v>0.13491156000000001</v>
       </c>
-      <c r="F16" s="16"/>
+      <c r="F16" s="65">
+        <v>0.14381029000000001</v>
+      </c>
       <c r="G16" s="45">
         <v>4.6170115497600001E-2</v>
       </c>
@@ -1519,10 +1558,12 @@
       <c r="D17" s="40">
         <v>0.11227771665400001</v>
       </c>
-      <c r="E17" s="57">
+      <c r="E17" s="50">
         <v>0.117693142446</v>
       </c>
-      <c r="F17" s="12"/>
+      <c r="F17" s="66">
+        <v>0.13467647448200001</v>
+      </c>
       <c r="G17" s="46">
         <v>9.5198856168199994E-2</v>
       </c>
@@ -1546,10 +1587,12 @@
       <c r="D18" s="40">
         <v>-7.1482368162699997E-2</v>
       </c>
-      <c r="E18" s="57">
+      <c r="E18" s="50">
         <v>-7.7746089016799996E-2</v>
       </c>
-      <c r="F18" s="12"/>
+      <c r="F18" s="66">
+        <v>-0.10422352477000001</v>
+      </c>
       <c r="G18" s="46">
         <v>0.36300457144600001</v>
       </c>
@@ -1573,10 +1616,12 @@
       <c r="D19" s="41">
         <v>2.0876598874899999E-2</v>
       </c>
-      <c r="E19" s="62">
+      <c r="E19" s="55">
         <v>1.8186120736899999E-2</v>
       </c>
-      <c r="F19" s="12"/>
+      <c r="F19" s="66">
+        <v>2.03596583395E-2</v>
+      </c>
       <c r="G19" s="46">
         <v>2.3044249287099999E-2</v>
       </c>
@@ -1600,10 +1645,12 @@
       <c r="D20" s="40">
         <v>1.8959050098099998E-2</v>
       </c>
-      <c r="E20" s="57">
+      <c r="E20" s="50">
         <v>1.66486008633E-2</v>
       </c>
-      <c r="F20" s="12"/>
+      <c r="F20" s="66">
+        <v>1.8672755524700001E-2</v>
+      </c>
       <c r="G20" s="46">
         <v>1.98190123644E-2</v>
       </c>
@@ -1627,10 +1674,12 @@
       <c r="D21" s="40">
         <v>1.8172989473100001E-2</v>
       </c>
-      <c r="E21" s="58">
+      <c r="E21" s="51">
         <v>1.57842238641E-2</v>
       </c>
-      <c r="F21" s="19"/>
+      <c r="F21" s="67">
+        <v>1.78668834948E-2</v>
+      </c>
       <c r="G21" s="47">
         <v>1.86839073664E-2</v>
       </c>
@@ -1649,24 +1698,27 @@
         <v>12</v>
       </c>
       <c r="C22" s="43">
-        <f>SUM(C$16:C$18, C19)</f>
+        <f t="shared" ref="C22:E24" si="5">SUM(C$16:C$18, C19)</f>
         <v>0.56370793962450005</v>
       </c>
       <c r="D22" s="43">
-        <f>SUM(D$16:D$18, D19)</f>
+        <f t="shared" si="5"/>
         <v>0.19387613736620002</v>
       </c>
       <c r="E22" s="43">
-        <f>SUM(E$16:E$18, E19)</f>
+        <f t="shared" si="5"/>
         <v>0.19304473416610002</v>
       </c>
-      <c r="F22" s="28"/>
+      <c r="F22" s="43">
+        <f>SUM(F$16:F$18, F19)</f>
+        <v>0.19462289805150002</v>
+      </c>
       <c r="G22" s="42">
-        <f>SUM(G$16:G$18, G19)</f>
+        <f t="shared" ref="G22:H24" si="6">SUM(G$16:G$18, G19)</f>
         <v>0.52741779239889997</v>
       </c>
       <c r="H22" s="42">
-        <f>SUM(H$16:H$18, H19)</f>
+        <f t="shared" si="6"/>
         <v>0.1017750678246</v>
       </c>
       <c r="I22" s="27"/>
@@ -1681,24 +1733,27 @@
         <v>13</v>
       </c>
       <c r="C23" s="43">
-        <f>SUM(C$16:C$18, C20)</f>
+        <f t="shared" si="5"/>
         <v>0.56050960762860003</v>
       </c>
       <c r="D23" s="43">
-        <f>SUM(D$16:D$18, D20)</f>
+        <f t="shared" si="5"/>
         <v>0.19195858858940001</v>
       </c>
       <c r="E23" s="43">
-        <f>SUM(E$16:E$18, E20)</f>
+        <f t="shared" si="5"/>
         <v>0.19150721429250003</v>
       </c>
-      <c r="F23" s="31"/>
+      <c r="F23" s="43">
+        <f t="shared" ref="F23" si="7">SUM(F$16:F$18, F20)</f>
+        <v>0.19293599523670002</v>
+      </c>
       <c r="G23" s="42">
-        <f>SUM(G$16:G$18, G20)</f>
+        <f t="shared" si="6"/>
         <v>0.52419255547619992</v>
       </c>
       <c r="H23" s="42">
-        <f>SUM(H$16:H$18, H20)</f>
+        <f t="shared" si="6"/>
         <v>9.9873160614099996E-2</v>
       </c>
       <c r="I23" s="21"/>
@@ -1713,24 +1768,27 @@
         <v>14</v>
       </c>
       <c r="C24" s="44">
-        <f>SUM(C$16:C$18, C21)</f>
+        <f t="shared" si="5"/>
         <v>0.55937943027920001</v>
       </c>
       <c r="D24" s="44">
-        <f>SUM(D$16:D$18, D21)</f>
+        <f t="shared" si="5"/>
         <v>0.19117252796440001</v>
       </c>
       <c r="E24" s="44">
-        <f>SUM(E$16:E$18, E21)</f>
+        <f t="shared" si="5"/>
         <v>0.19064283729330003</v>
       </c>
-      <c r="F24" s="30"/>
+      <c r="F24" s="44">
+        <f t="shared" ref="F24" si="8">SUM(F$16:F$18, F21)</f>
+        <v>0.19213012320680004</v>
+      </c>
       <c r="G24" s="48">
-        <f>SUM(G$16:G$18, G21)</f>
+        <f t="shared" si="6"/>
         <v>0.52305745047819996</v>
       </c>
       <c r="H24" s="48">
-        <f>SUM(H$16:H$18, H21)</f>
+        <f t="shared" si="6"/>
         <v>9.9091012516200005E-2</v>
       </c>
       <c r="I24" s="29"/>
@@ -1743,25 +1801,23 @@
     <row r="25" spans="2:22" x14ac:dyDescent="0.35">
       <c r="C25" s="3"/>
       <c r="D25" s="38"/>
-      <c r="F25" s="3"/>
       <c r="G25" s="3"/>
       <c r="M25" s="3"/>
     </row>
     <row r="26" spans="2:22" x14ac:dyDescent="0.35">
       <c r="C26" s="3"/>
       <c r="D26" s="38"/>
-      <c r="F26" s="3"/>
       <c r="G26" s="3"/>
     </row>
     <row r="27" spans="2:22" x14ac:dyDescent="0.35">
-      <c r="O27" s="49"/>
-      <c r="P27" s="49"/>
-      <c r="Q27" s="49"/>
-      <c r="R27" s="49"/>
-      <c r="S27" s="49"/>
-      <c r="T27" s="49"/>
-      <c r="U27" s="49"/>
-      <c r="V27" s="49"/>
+      <c r="O27" s="61"/>
+      <c r="P27" s="61"/>
+      <c r="Q27" s="61"/>
+      <c r="R27" s="61"/>
+      <c r="S27" s="61"/>
+      <c r="T27" s="61"/>
+      <c r="U27" s="61"/>
+      <c r="V27" s="61"/>
     </row>
     <row r="29" spans="2:22" x14ac:dyDescent="0.35">
       <c r="O29" s="3"/>
@@ -1821,21 +1877,20 @@
       <c r="C35" s="3"/>
       <c r="D35" s="38"/>
       <c r="E35" s="3"/>
-      <c r="F35" s="3"/>
       <c r="G35" s="3"/>
     </row>
   </sheetData>
   <mergeCells count="10">
+    <mergeCell ref="O27:R27"/>
+    <mergeCell ref="S27:V27"/>
+    <mergeCell ref="M2:P2"/>
+    <mergeCell ref="C14:F14"/>
+    <mergeCell ref="M4:M5"/>
     <mergeCell ref="B2:B3"/>
     <mergeCell ref="B14:B15"/>
     <mergeCell ref="G14:J14"/>
     <mergeCell ref="C2:F2"/>
     <mergeCell ref="G2:J2"/>
-    <mergeCell ref="O27:R27"/>
-    <mergeCell ref="S27:V27"/>
-    <mergeCell ref="M2:P2"/>
-    <mergeCell ref="C14:F14"/>
-    <mergeCell ref="M4:M5"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>

</xml_diff>